<commit_message>
Fix Monster Add Animation
</commit_message>
<xml_diff>
--- a/test1/GlobalConfig.xlsx
+++ b/test1/GlobalConfig.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitPjt\ExcelAndJSON\test1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
+    <workbookView windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConfig" sheetId="1" r:id="rId1"/>
@@ -27,40 +22,42 @@
     <t>__type__</t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>i</t>
   </si>
   <si>
     <t>__name__</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>AttackLiteImpactRatio</t>
   </si>
   <si>
-    <t>MID</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>AttackHeavyImpactRatio</t>
   </si>
   <si>
     <t>ViewAngle</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>MinRange</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -68,39 +65,360 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -108,9 +426,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -128,20 +688,64 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -155,7 +759,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="E0FFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -399,36 +1003,39 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6636363636364" defaultRowHeight="14.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="16375" width="15.6640625" style="2" customWidth="1"/>
-    <col min="16376" max="16384" width="15.6640625" style="2"/>
+    <col min="1" max="1" width="15.6636363636364" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.3636363636364" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.3636363636364" style="2" customWidth="1"/>
+    <col min="4" max="16375" width="15.6636363636364" style="2" customWidth="1"/>
+    <col min="16376" max="16384" width="15.6636363636364" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.5" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E1" s="3">
         <v>1</v>
@@ -438,7 +1045,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" s="1" customFormat="1" ht="14" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -449,30 +1056,30 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="1" customFormat="1" ht="15.5" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -490,7 +1097,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>